<commit_message>
ajouté # de pièces option 2 de connectgeur batterie 9V
</commit_message>
<xml_diff>
--- a/Releases/Main Board - R1.1/BOM - Non jlcpcb - Ceinture_respiration_Main.xlsx
+++ b/Releases/Main Board - R1.1/BOM - Non jlcpcb - Ceinture_respiration_Main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\PCB\AT-CeintureRespiration\Releases\Main Board - R1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0663B918-B47A-433E-B53B-778BE5E50298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56279BAB-D69F-4797-9751-2F310F0494BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{5A351B18-678D-45CE-883B-00C33A0DE58B}"/>
+    <workbookView xWindow="240" yWindow="1755" windowWidth="29040" windowHeight="13305" xr2:uid="{5A351B18-678D-45CE-883B-00C33A0DE58B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ceinture_respiration_Main" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>BT1</t>
   </si>
   <si>
-    <t>BH9VPC</t>
-  </si>
-  <si>
     <t>Excluded from BOM</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>Arduinon nano 33 ble R2</t>
+  </si>
+  <si>
+    <t>BH9VPC / 36-232-ND</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1018,72 +1018,72 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>